<commit_message>
Redid IsopyKeyList. Now there is only one list type that contains the keys.
Rewrote the flavour implementation to allow better comparisons
</commit_message>
<xml_diff>
--- a/tests/files/test_io1.xlsx
+++ b/tests/files/test_io1.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="test_sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="test_sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,104 +440,35 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>11.1</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>21.1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12.2</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C3" t="n">
-        <v>22.2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>13.3</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>23.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Pd</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Cd</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Ru</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>21.1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12.2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>23.3</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>